<commit_message>
Added auto|fixed|cutstom column size
</commit_message>
<xml_diff>
--- a/CsvToXlsx/bin/Debug/combined.xlsx
+++ b/CsvToXlsx/bin/Debug/combined.xlsx
@@ -990,7 +990,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
@@ -1005,6 +1005,7 @@
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="4" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="1" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,9 +1024,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="100" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="2">
       <c r="A2" s="0" t="s">
@@ -1321,8 +1319,8 @@
       <c r="G18" s="12">
         <v>2.9</v>
       </c>
-      <c r="H18" s="12">
-        <v>812</v>
+      <c r="H18" s="14">
+        <v>0</v>
       </c>
       <c r="I18" s="0" t="s">
         <v>0</v>

</xml_diff>